<commit_message>
Power function (mV to W)
</commit_message>
<xml_diff>
--- a/mV_to_power_mapping - 20A - 1Mohm.xlsx
+++ b/mV_to_power_mapping - 20A - 1Mohm.xlsx
@@ -13,10 +13,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1681497366" val="1062" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1681497366" showFormulas="1" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1681497366" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1681497366"/>
+      <pm:revision xmlns:pm="smNativeData" day="1681537630" val="1062" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1681537630" showFormulas="1" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1681537630" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1681537630"/>
     </ext>
   </extLst>
 </workbook>
@@ -28,10 +28,10 @@
     <t>No</t>
   </si>
   <si>
-    <t>Measured Watts [W]</t>
+    <t>Measured Voltage [mV]</t>
   </si>
   <si>
-    <t>Measured Voltage [mV]</t>
+    <t>Measured Watts [W]</t>
   </si>
 </sst>
 </file>
@@ -56,7 +56,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1681497366" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1681537630" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -72,7 +72,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1681497366" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1681537630" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -81,7 +81,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,45 +89,10 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1681497366" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
       <patternFill patternType="none"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -143,198 +108,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681497366"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681497366"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681497366">
-            <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-            <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-          </pm:border>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681497366">
-            <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-          </pm:border>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681497366">
-            <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-            <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-          </pm:border>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681497366">
-            <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-          </pm:border>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681497366">
-            <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-          </pm:border>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681497366">
-            <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-            <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-          </pm:border>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681497366">
-            <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-          </pm:border>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681497366">
-            <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-            <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-          </pm:border>
+          <pm:border xmlns:pm="smNativeData" id="1681537630"/>
         </ext>
       </extLst>
     </border>
@@ -353,7 +127,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681497366">
+          <pm:border xmlns:pm="smNativeData" id="1681537630">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -368,10 +142,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -379,7 +153,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1681497366" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1681537630" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -414,16 +188,22 @@
           <c:order val="0"/>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-us" sz="1000" b="0" i="0" u="none" strike="noStrike">
+                  <a:defRPr lang="en-us" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="100">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="Arial"/>
+                    <a:latin typeface="Arial" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
@@ -450,16 +230,22 @@
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c:spPr>
               <c:txPr>
                 <a:bodyPr/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr lang="en-us" sz="1000" b="0" i="0" u="none" strike="noStrike">
+                    <a:defRPr lang="en-us" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="100">
                       <a:solidFill>
                         <a:srgbClr val="000000"/>
                       </a:solidFill>
-                      <a:latin typeface="Arial"/>
+                      <a:latin typeface="Arial" charset="0"/>
                     </a:defRPr>
                   </a:pPr>
                 </a:p>
@@ -476,28 +262,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>400</c:v>
+                  <c:v>690</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>670</c:v>
+                  <c:v>1150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1130</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1340</c:v>
+                  <c:v>2340</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2460</c:v>
+                  <c:v>3860</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2460</c:v>
+                  <c:v>3860</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2460</c:v>
+                  <c:v>3860</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -512,28 +298,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>300</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>690</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1150</c:v>
+                  <c:v>670</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2000</c:v>
+                  <c:v>1130</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2340</c:v>
+                  <c:v>1340</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3860</c:v>
+                  <c:v>2460</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3860</c:v>
+                  <c:v>2460</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3860</c:v>
+                  <c:v>2460</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -543,28 +329,28 @@
             <c:ext xmlns:sm="smo" uri="smo">
               <sm:meanLine>
                 <c:spPr>
-                  <a:ln>
+                  <a:ln w="9525">
                     <a:noFill/>
                   </a:ln>
                 </c:spPr>
               </sm:meanLine>
               <sm:minMaxLine>
                 <c:spPr>
-                  <a:ln>
+                  <a:ln w="9525">
                     <a:noFill/>
                   </a:ln>
                 </c:spPr>
               </sm:minMaxLine>
               <sm:stDevLine>
                 <c:spPr>
-                  <a:ln>
+                  <a:ln w="9525">
                     <a:noFill/>
                   </a:ln>
                 </c:spPr>
               </sm:stDevLine>
               <sm:trendLine>
                 <c:spPr>
-                  <a:ln>
+                  <a:ln w="9525">
                     <a:noFill/>
                   </a:ln>
                 </c:spPr>
@@ -627,6 +413,11 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
       <c:txPr>
         <a:bodyPr anchor="t"/>
         <a:lstStyle/>
@@ -646,18 +437,18 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr lang="en-us" sz="2510" b="0" i="0" u="none" strike="noStrike">
+        <a:defRPr lang="en-us" sz="2510" b="0" i="0" u="none" strike="noStrike" kern="100">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
-          <a:latin typeface="Arial"/>
+          <a:latin typeface="Arial" charset="0"/>
         </a:defRPr>
       </a:pPr>
     </a:p>
   </c:txPr>
   <c:extLst>
     <c:ext xmlns:sm="smo" uri="smo">
-      <sm:colorScheme xmlns:sm="smo" id="1681497366" val="7"/>
+      <sm:colorScheme xmlns:sm="smo" id="1681537630" val="7"/>
     </c:ext>
   </c:extLst>
 </c:chartSpace>
@@ -954,19 +745,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
-    <col min="2" max="2" width="11.774775" customWidth="1"/>
+    <col min="2" max="2" width="16.819820" customWidth="1"/>
     <col min="3" max="3" width="14.684685" customWidth="1"/>
+    <col min="4" max="4" width="16.819820" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="36.95" customHeight="1">
+    <row r="1" spans="1:4" ht="36.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -976,8 +768,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
@@ -987,92 +780,101 @@
       <c r="C2" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>300</v>
-      </c>
+      <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="n">
+        <v>690</v>
+      </c>
+      <c r="C4" s="2" t="n">
         <v>400</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>690</v>
-      </c>
+      <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="n">
+        <v>1150</v>
+      </c>
+      <c r="C5" s="2" t="n">
         <v>670</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>1150</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C6" s="2" t="n">
         <v>1130</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>2000</v>
-      </c>
+      <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="n">
+        <v>2340</v>
+      </c>
+      <c r="C7" s="2" t="n">
         <v>1340</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>2340</v>
-      </c>
+      <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="n">
+        <v>3860</v>
+      </c>
+      <c r="C8" s="2" t="n">
         <v>2460</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>3860</v>
-      </c>
+      <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1681497366" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1681537630" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1081,17 +883,17 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1681497366" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1681497366" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1681497366" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1681497366" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1681537630" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1681537630" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1681537630" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1681537630" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <drawing r:id="rId1"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1681497366" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1681537630" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>